<commit_message>
Updating England location names in LA .xlsx, re-running wide to long .qmd, updating bds_long dataset and renv
</commit_message>
<xml_diff>
--- a/01_data/02_prod/LA code list.xlsx
+++ b/01_data/02_prod/LA code list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtufts\Documents\no_net_work\Projects\Main projects\lait-shiny\01_data\02_prod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtufts\Documents\no_net_work\Open source\local-authority-interactive-tool\01_data\02_prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F28C39-D572-4EE6-81C9-F397559BBF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29EF1C3-6317-4C8A-B499-977CC6BFF99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{705009BA-2E1E-4365-A1C7-A05A8D2FB56B}"/>
+    <workbookView xWindow="-20865" yWindow="-21765" windowWidth="38640" windowHeight="21120" xr2:uid="{705009BA-2E1E-4365-A1C7-A05A8D2FB56B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -584,17 +584,17 @@
     <t>London (Outer)</t>
   </si>
   <si>
-    <t>England_state_funded</t>
-  </si>
-  <si>
-    <t>England_all_schools</t>
+    <t>England (State-funded)</t>
+  </si>
+  <si>
+    <t>England (All schools)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,12 +624,6 @@
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="MS Sans Serif"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1014,7 +1008,7 @@
   <dimension ref="A1:D172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="H169" sqref="H169"/>
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Data: Updating data for new BDS, aligning LA names across LA code list and SN
</commit_message>
<xml_diff>
--- a/01_data/02_prod/LA code list.xlsx
+++ b/01_data/02_prod/LA code list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtufts\Documents\no_net_work\Open source\local-authority-interactive-tool\01_data\02_prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29EF1C3-6317-4C8A-B499-977CC6BFF99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CCFF86-D60E-4566-BC8F-92849C234EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20865" yWindow="-21765" windowWidth="38640" windowHeight="21120" xr2:uid="{705009BA-2E1E-4365-A1C7-A05A8D2FB56B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{705009BA-2E1E-4365-A1C7-A05A8D2FB56B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -545,15 +545,9 @@
     <t>Bournemouth (Pre LG)</t>
   </si>
   <si>
-    <t>Bournemouth, Christ Church and Poole</t>
-  </si>
-  <si>
     <t>Bristol, City of</t>
   </si>
   <si>
-    <t>Westmoreland and Furness</t>
-  </si>
-  <si>
     <t>Dorset (Pre LG)</t>
   </si>
   <si>
@@ -584,10 +578,16 @@
     <t>London (Outer)</t>
   </si>
   <si>
-    <t>England (State-funded)</t>
-  </si>
-  <si>
-    <t>England (All schools)</t>
+    <t>England</t>
+  </si>
+  <si>
+    <t>England (discontinued)</t>
+  </si>
+  <si>
+    <t>Westmorland and Furness</t>
+  </si>
+  <si>
+    <t>Bournemouth, Christchurch and Poole</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B552FD6-2159-46B1-9E1B-8283F3E2C43B}">
   <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,10 +1025,10 @@
         <v>161</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1190,7 +1190,7 @@
         <v>839</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1260,7 +1260,7 @@
         <v>801</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1484,7 +1484,7 @@
         <v>943</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
@@ -1568,7 +1568,7 @@
         <v>835</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1974,7 +1974,7 @@
         <v>810</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
@@ -2478,7 +2478,7 @@
         <v>836</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
@@ -3248,13 +3248,13 @@
         <v>970</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C160" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D160" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
@@ -3265,10 +3265,10 @@
         <v>38</v>
       </c>
       <c r="C161" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D161" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
@@ -3279,10 +3279,10 @@
         <v>14</v>
       </c>
       <c r="C162" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D162" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
@@ -3290,13 +3290,13 @@
         <v>982</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C163" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D163" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
@@ -3307,10 +3307,10 @@
         <v>40</v>
       </c>
       <c r="C164" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D164" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
@@ -3321,10 +3321,10 @@
         <v>12</v>
       </c>
       <c r="C165" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D165" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
@@ -3335,10 +3335,10 @@
         <v>9</v>
       </c>
       <c r="C166" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D166" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
@@ -3346,13 +3346,13 @@
         <v>986</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C167" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D167" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
@@ -3360,13 +3360,13 @@
         <v>987</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C168" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D168" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
@@ -3374,13 +3374,13 @@
         <v>988</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C169" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D169" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
@@ -3391,10 +3391,10 @@
         <v>18</v>
       </c>
       <c r="C170" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D170" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
@@ -3405,10 +3405,10 @@
         <v>7</v>
       </c>
       <c r="C171" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D171" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
@@ -3416,13 +3416,13 @@
         <v>1000</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C172" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D172" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>